<commit_message>
Materialiste i Excel opdateret
</commit_message>
<xml_diff>
--- a/documents/Materialeliste beregninger.xlsx
+++ b/documents/Materialeliste beregninger.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bruger\Desktop\2 SEM eksamen\Fog\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19E5D8F8-3232-4784-BFD9-D66CB2EB6847}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CFBBDBD-D5E1-4932-8569-87FE3914AFC4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="5175" windowWidth="29040" windowHeight="15840" xr2:uid="{02919F5A-1519-4947-A4AE-EA2FF4BD8D19}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{02919F5A-1519-4947-A4AE-EA2FF4BD8D19}"/>
   </bookViews>
   <sheets>
     <sheet name="Alt" sheetId="1" r:id="rId1"/>
@@ -51,9 +51,6 @@
     <t>Uden</t>
   </si>
   <si>
-    <t>300 mm udhæng i hver ende og et bræt på hver side. Derfor starter værdien på 1200 mm.</t>
-  </si>
-  <si>
     <t>Med</t>
   </si>
   <si>
@@ -141,9 +138,6 @@
     <t>900 + carport højde</t>
   </si>
   <si>
-    <t>600 + carport længde</t>
-  </si>
-  <si>
     <t>((skur længde / 60) x 2) + ((skur bredde / 60) x 2))</t>
   </si>
   <si>
@@ -445,6 +439,12 @@
   </si>
   <si>
     <t>Trapez plast sort</t>
+  </si>
+  <si>
+    <t>300 + carport længde</t>
+  </si>
+  <si>
+    <t>300 mm udhæng i hver ende og et bræt på hver side.</t>
   </si>
 </sst>
 </file>
@@ -871,7 +871,7 @@
   <dimension ref="A1:L47"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A46" sqref="A46"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -883,7 +883,7 @@
     <col min="5" max="5" width="7.44140625" style="1" customWidth="1"/>
     <col min="6" max="6" width="14.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="44.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="24.88671875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="35.5546875" style="1" customWidth="1"/>
     <col min="9" max="9" width="22.77734375" style="1" customWidth="1"/>
     <col min="10" max="10" width="75.5546875" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="13" style="1" customWidth="1"/>
@@ -908,7 +908,7 @@
     <row r="2" spans="1:12" s="7" customFormat="1" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6"/>
       <c r="B2" s="15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C2" s="15"/>
       <c r="D2" s="15"/>
@@ -924,37 +924,37 @@
     <row r="3" spans="1:12" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6"/>
       <c r="B3" s="14" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G3" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="8" t="s">
-        <v>8</v>
-      </c>
       <c r="I3" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="J3" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="J3" s="8" t="s">
-        <v>33</v>
-      </c>
       <c r="K3" s="8" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="L3" s="8" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="4" spans="1:12" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -972,16 +972,16 @@
         <v>1</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H4" s="9" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="I4" s="9" t="s">
-        <v>35</v>
+        <v>135</v>
       </c>
       <c r="J4" s="9">
         <v>2</v>
@@ -990,7 +990,7 @@
         <v>3</v>
       </c>
       <c r="L4" s="9" t="s">
-        <v>5</v>
+        <v>136</v>
       </c>
     </row>
     <row r="5" spans="1:12" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1008,16 +1008,16 @@
         <v>1</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H5" s="9" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="I5" s="9" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="J5" s="9">
         <v>1</v>
@@ -1035,7 +1035,7 @@
         <v>3</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D6" s="9" t="s">
         <v>1</v>
@@ -1044,16 +1044,16 @@
         <v>4</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G6" s="9" t="s">
         <v>0</v>
       </c>
       <c r="H6" s="9" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="I6" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J6" s="9">
         <v>4</v>
@@ -1062,7 +1062,7 @@
         <v>3</v>
       </c>
       <c r="L6" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:12" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1071,7 +1071,7 @@
         <v>3</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D7" s="9" t="s">
         <v>1</v>
@@ -1080,16 +1080,16 @@
         <v>4</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G7" s="9" t="s">
         <v>0</v>
       </c>
       <c r="H7" s="9" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="I7" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J7" s="9">
         <v>6</v>
@@ -1098,7 +1098,7 @@
         <v>3</v>
       </c>
       <c r="L7" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:12" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1113,19 +1113,19 @@
         <v>1</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G8" s="9" t="s">
         <v>0</v>
       </c>
       <c r="H8" s="9" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="I8" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J8" s="9">
         <v>10</v>
@@ -1134,7 +1134,7 @@
         <v>3</v>
       </c>
       <c r="L8" s="9" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="9" spans="1:12" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1149,28 +1149,28 @@
         <v>1</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H9" s="9" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="I9" s="9" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="J9" s="10" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="K9" s="9" t="s">
         <v>3</v>
       </c>
       <c r="L9" s="9" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="10" spans="1:12" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1185,16 +1185,16 @@
         <v>1</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G10" s="9" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="H10" s="9" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="I10" s="9">
         <v>420</v>
@@ -1224,16 +1224,16 @@
         <v>1</v>
       </c>
       <c r="F11" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="G11" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="H11" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="I11" s="9" t="s">
         <v>47</v>
-      </c>
-      <c r="G11" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="H11" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="I11" s="9" t="s">
-        <v>49</v>
       </c>
       <c r="J11" s="9">
         <v>2</v>
@@ -1260,25 +1260,25 @@
         <v>1</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="H12" s="9" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="I12" s="9" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="J12" s="9" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="K12" s="9" t="s">
         <v>3</v>
       </c>
       <c r="L12" s="9" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="13" spans="1:12" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1293,19 +1293,19 @@
         <v>1</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G13" s="9" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="H13" s="9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="I13" s="9" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="J13" s="9">
         <v>2</v>
@@ -1314,7 +1314,7 @@
         <v>3</v>
       </c>
       <c r="L13" s="9" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="14" spans="1:12" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1329,19 +1329,19 @@
         <v>1</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G14" s="9" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="H14" s="9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="I14" s="9" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="J14" s="9">
         <v>2</v>
@@ -1350,7 +1350,7 @@
         <v>3</v>
       </c>
       <c r="L14" s="9" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="15" spans="1:12" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1362,31 +1362,31 @@
         <v>3</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E15" s="9" t="s">
         <v>1</v>
       </c>
       <c r="F15" s="9" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G15" s="9" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="H15" s="9" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="I15" s="9">
         <v>0</v>
       </c>
       <c r="J15" s="9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="K15" s="9" t="s">
         <v>3</v>
       </c>
       <c r="L15" s="9" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:12" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1398,22 +1398,22 @@
         <v>3</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E16" s="9" t="s">
         <v>1</v>
       </c>
       <c r="F16" s="9" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G16" s="9" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="H16" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="I16" s="9" t="s">
         <v>122</v>
-      </c>
-      <c r="I16" s="9" t="s">
-        <v>124</v>
       </c>
       <c r="J16" s="9">
         <v>2</v>
@@ -1422,7 +1422,7 @@
         <v>3</v>
       </c>
       <c r="L16" s="9" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="17" spans="1:12" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1434,31 +1434,31 @@
         <v>3</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E17" s="9" t="s">
         <v>1</v>
       </c>
       <c r="F17" s="9" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G17" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="H17" s="9" t="s">
         <v>125</v>
-      </c>
-      <c r="H17" s="9" t="s">
-        <v>127</v>
       </c>
       <c r="I17" s="9">
         <v>540</v>
       </c>
       <c r="J17" s="9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="K17" s="9" t="s">
         <v>3</v>
       </c>
       <c r="L17" s="9" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="18" spans="1:12" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1470,23 +1470,23 @@
         <v>3</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E18" s="9" t="s">
         <v>1</v>
       </c>
       <c r="F18" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="G18" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="H18" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="I18" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="G18" s="9" t="s">
-        <v>125</v>
-      </c>
-      <c r="H18" s="9" t="s">
-        <v>128</v>
-      </c>
-      <c r="I18" s="9" t="s">
-        <v>49</v>
-      </c>
       <c r="J18" s="9">
         <v>1</v>
       </c>
@@ -1494,7 +1494,7 @@
         <v>3</v>
       </c>
       <c r="L18" s="9" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="19" spans="1:12" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1512,25 +1512,25 @@
         <v>1</v>
       </c>
       <c r="F19" s="9" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G19" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H19" s="9" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="I19" s="9" t="s">
         <v>3</v>
       </c>
       <c r="J19" s="9" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="K19" s="9" t="s">
         <v>3</v>
       </c>
       <c r="L19" s="9" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="20" spans="1:12" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1542,31 +1542,31 @@
         <v>3</v>
       </c>
       <c r="D20" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E20" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="F20" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="G20" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="E20" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="F20" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="G20" s="9" t="s">
+      <c r="H20" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="I20" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="J20" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="K20" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="L20" s="9" t="s">
         <v>21</v>
-      </c>
-      <c r="H20" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="I20" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="J20" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="K20" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="L20" s="9" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="21" spans="1:12" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1578,31 +1578,31 @@
         <v>3</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E21" s="9" t="s">
         <v>1</v>
       </c>
       <c r="F21" s="9" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G21" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="H21" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="H21" s="9" t="s">
-        <v>24</v>
-      </c>
       <c r="I21" s="9" t="s">
         <v>3</v>
       </c>
       <c r="J21" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K21" s="9" t="s">
         <v>3</v>
       </c>
       <c r="L21" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="22" spans="1:12" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1614,31 +1614,31 @@
         <v>3</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E22" s="9" t="s">
         <v>1</v>
       </c>
       <c r="F22" s="9" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G22" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H22" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I22" s="9" t="s">
         <v>3</v>
       </c>
       <c r="J22" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K22" s="9" t="s">
         <v>3</v>
       </c>
       <c r="L22" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="23" spans="1:12" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1647,7 +1647,7 @@
         <v>18</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D23" s="9" t="s">
         <v>2</v>
@@ -1656,25 +1656,25 @@
         <v>1</v>
       </c>
       <c r="F23" s="9" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G23" s="9" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="H23" s="9" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I23" s="9" t="s">
         <v>3</v>
       </c>
       <c r="J23" s="9" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="K23" s="9" t="s">
         <v>3</v>
       </c>
       <c r="L23" s="9" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="24" spans="1:12" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1686,31 +1686,31 @@
         <v>3</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E24" s="9" t="s">
         <v>1</v>
       </c>
       <c r="F24" s="9" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G24" s="9" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="H24" s="9" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="I24" s="9" t="s">
         <v>3</v>
       </c>
       <c r="J24" s="9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="K24" s="9" t="s">
         <v>3</v>
       </c>
       <c r="L24" s="9" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="25" spans="1:12" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1722,31 +1722,31 @@
         <v>3</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E25" s="9" t="s">
         <v>1</v>
       </c>
       <c r="F25" s="9" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G25" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="H25" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="I25" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="J25" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="K25" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="L25" s="9" t="s">
         <v>115</v>
-      </c>
-      <c r="H25" s="9" t="s">
-        <v>116</v>
-      </c>
-      <c r="I25" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="J25" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="K25" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="L25" s="9" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="26" spans="1:12" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1758,31 +1758,31 @@
         <v>3</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E26" s="9" t="s">
         <v>1</v>
       </c>
       <c r="F26" s="9" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G26" s="9" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="H26" s="9" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="I26" s="9" t="s">
         <v>3</v>
       </c>
       <c r="J26" s="9" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="K26" s="9" t="s">
         <v>3</v>
       </c>
       <c r="L26" s="9" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="27" spans="1:12" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1800,25 +1800,25 @@
         <v>1</v>
       </c>
       <c r="F27" s="9" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G27" s="9" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H27" s="9" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="I27" s="9" t="s">
         <v>3</v>
       </c>
       <c r="J27" s="9" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="K27" s="9" t="s">
         <v>3</v>
       </c>
       <c r="L27" s="9" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="28" spans="1:12" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1836,25 +1836,25 @@
         <v>1</v>
       </c>
       <c r="F28" s="9" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G28" s="9" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="H28" s="9" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="I28" s="9" t="s">
         <v>3</v>
       </c>
       <c r="J28" s="9" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="K28" s="9" t="s">
         <v>3</v>
       </c>
       <c r="L28" s="9" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="29" spans="1:12" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1872,25 +1872,25 @@
         <v>1</v>
       </c>
       <c r="F29" s="9" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G29" s="9" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="H29" s="9" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="I29" s="9" t="s">
         <v>3</v>
       </c>
       <c r="J29" s="9" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="K29" s="9" t="s">
         <v>3</v>
       </c>
       <c r="L29" s="9" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="30" spans="1:12" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1908,25 +1908,25 @@
         <v>1</v>
       </c>
       <c r="F30" s="9" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G30" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="H30" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="I30" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="J30" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="H30" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="I30" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="J30" s="9" t="s">
-        <v>84</v>
-      </c>
       <c r="K30" s="9" t="s">
         <v>3</v>
       </c>
       <c r="L30" s="9" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="31" spans="1:12" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1935,7 +1935,7 @@
         <v>26</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D31" s="9" t="s">
         <v>1</v>
@@ -1944,13 +1944,13 @@
         <v>4</v>
       </c>
       <c r="F31" s="9" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G31" s="9" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="H31" s="9" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="I31" s="9" t="s">
         <v>3</v>
@@ -1962,7 +1962,7 @@
         <v>3</v>
       </c>
       <c r="L31" s="9" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="32" spans="1:12" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1971,7 +1971,7 @@
         <v>26</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D32" s="9" t="s">
         <v>1</v>
@@ -1980,13 +1980,13 @@
         <v>4</v>
       </c>
       <c r="F32" s="9" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G32" s="9" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="H32" s="9" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="I32" s="9" t="s">
         <v>3</v>
@@ -1998,7 +1998,7 @@
         <v>3</v>
       </c>
       <c r="L32" s="9" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="33" spans="1:12" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -2013,16 +2013,16 @@
         <v>1</v>
       </c>
       <c r="E33" s="9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F33" s="9" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G33" s="9" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="H33" s="9" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="I33" s="9" t="s">
         <v>3</v>
@@ -2034,7 +2034,7 @@
         <v>3</v>
       </c>
       <c r="L33" s="9" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="34" spans="1:12" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -2043,7 +2043,7 @@
         <v>27</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D34" s="9" t="s">
         <v>1</v>
@@ -2052,13 +2052,13 @@
         <v>4</v>
       </c>
       <c r="F34" s="9" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G34" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="H34" s="9" t="s">
         <v>72</v>
-      </c>
-      <c r="H34" s="9" t="s">
-        <v>74</v>
       </c>
       <c r="I34" s="9" t="s">
         <v>3</v>
@@ -2070,7 +2070,7 @@
         <v>3</v>
       </c>
       <c r="L34" s="9" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="35" spans="1:12" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -2079,7 +2079,7 @@
         <v>27</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D35" s="9" t="s">
         <v>1</v>
@@ -2088,13 +2088,13 @@
         <v>4</v>
       </c>
       <c r="F35" s="9" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G35" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="H35" s="9" t="s">
         <v>72</v>
-      </c>
-      <c r="H35" s="9" t="s">
-        <v>74</v>
       </c>
       <c r="I35" s="9" t="s">
         <v>3</v>
@@ -2106,7 +2106,7 @@
         <v>3</v>
       </c>
       <c r="L35" s="9" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="36" spans="1:12" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -2121,16 +2121,16 @@
         <v>1</v>
       </c>
       <c r="E36" s="9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F36" s="9" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G36" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="H36" s="9" t="s">
         <v>72</v>
-      </c>
-      <c r="H36" s="9" t="s">
-        <v>74</v>
       </c>
       <c r="I36" s="9" t="s">
         <v>3</v>
@@ -2142,7 +2142,7 @@
         <v>3</v>
       </c>
       <c r="L36" s="9" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="37" spans="1:12" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -2160,25 +2160,25 @@
         <v>1</v>
       </c>
       <c r="F37" s="9" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G37" s="9" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H37" s="9" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="I37" s="9" t="s">
         <v>3</v>
       </c>
       <c r="J37" s="9" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="K37" s="9" t="s">
         <v>3</v>
       </c>
       <c r="L37" s="9" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="38" spans="1:12" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -2193,16 +2193,16 @@
         <v>1</v>
       </c>
       <c r="E38" s="9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F38" s="9" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G38" s="9" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="H38" s="9" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="I38" s="9" t="s">
         <v>3</v>
@@ -2229,16 +2229,16 @@
         <v>1</v>
       </c>
       <c r="E39" s="9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F39" s="9" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G39" s="9" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H39" s="9" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="I39" s="9" t="s">
         <v>3</v>
@@ -2265,28 +2265,28 @@
         <v>1</v>
       </c>
       <c r="E40" s="9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F40" s="9" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G40" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="H40" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="I40" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="J40" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="K40" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="L40" s="9" t="s">
         <v>99</v>
-      </c>
-      <c r="H40" s="9" t="s">
-        <v>100</v>
-      </c>
-      <c r="I40" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="J40" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="K40" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="L40" s="9" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="41" spans="1:12" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -2301,28 +2301,28 @@
         <v>1</v>
       </c>
       <c r="E41" s="9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F41" s="9" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G41" s="9" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="H41" s="9" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="I41" s="9" t="s">
         <v>3</v>
       </c>
       <c r="J41" s="10" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="K41" s="9" t="s">
         <v>3</v>
       </c>
       <c r="L41" s="9" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="42" spans="1:12" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -2337,28 +2337,28 @@
         <v>1</v>
       </c>
       <c r="E42" s="9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F42" s="9" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G42" s="9" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="H42" s="9" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="I42" s="9" t="s">
         <v>3</v>
       </c>
       <c r="J42" s="10" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="K42" s="9" t="s">
         <v>3</v>
       </c>
       <c r="L42" s="9" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="43" spans="1:12" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -2376,25 +2376,25 @@
         <v>1</v>
       </c>
       <c r="F43" s="9" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G43" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H43" s="9" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="I43" s="9" t="s">
         <v>3</v>
       </c>
       <c r="J43" s="9" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="K43" s="9" t="s">
         <v>3</v>
       </c>
       <c r="L43" s="9" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="44" spans="1:12" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -2412,25 +2412,25 @@
         <v>1</v>
       </c>
       <c r="F44" s="9" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G44" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H44" s="9" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="I44" s="9" t="s">
         <v>3</v>
       </c>
       <c r="J44" s="9" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="K44" s="9" t="s">
         <v>3</v>
       </c>
       <c r="L44" s="9" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="45" spans="1:12" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -2448,25 +2448,25 @@
         <v>1</v>
       </c>
       <c r="F45" s="9" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G45" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H45" s="9" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="I45" s="9" t="s">
         <v>3</v>
       </c>
       <c r="J45" s="9" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="K45" s="9" t="s">
         <v>3</v>
       </c>
       <c r="L45" s="9" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="46" spans="1:12" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -2478,31 +2478,31 @@
         <v>3</v>
       </c>
       <c r="D46" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E46" s="9" t="s">
         <v>1</v>
       </c>
       <c r="F46" s="9" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G46" s="9" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="H46" s="9" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="I46" s="9" t="s">
         <v>3</v>
       </c>
       <c r="J46" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K46" s="9" t="s">
         <v>3</v>
       </c>
       <c r="L46" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="47" spans="1:12" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -2514,31 +2514,31 @@
         <v>3</v>
       </c>
       <c r="D47" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E47" s="9" t="s">
         <v>1</v>
       </c>
       <c r="F47" s="9" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G47" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H47" s="9" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="I47" s="9" t="s">
         <v>3</v>
       </c>
       <c r="J47" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K47" s="9" t="s">
         <v>3</v>
       </c>
       <c r="L47" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Materialiste i Excel, Calculator.java og diagrammer er opdateret.
</commit_message>
<xml_diff>
--- a/documents/Materialeliste beregninger.xlsx
+++ b/documents/Materialeliste beregninger.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bruger\Desktop\2 SEM eksamen\Fog\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CFBBDBD-D5E1-4932-8569-87FE3914AFC4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8504F5E4-D5F5-44A4-9A99-7A0DE3F5A886}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{02919F5A-1519-4947-A4AE-EA2FF4BD8D19}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Alt" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Alt!$B$3:$L$47</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Alt!$B$3:$K$47</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="139">
   <si>
     <t>Stolpe</t>
   </si>
@@ -72,12 +72,6 @@
     <t>Tagtype</t>
   </si>
   <si>
-    <t>Carport længde &gt; 4800</t>
-  </si>
-  <si>
-    <t>Carport længde &lt; 4800</t>
-  </si>
-  <si>
     <t xml:space="preserve">4 stolper pr. skur. 900 mm nedgravet pr. stolpe. </t>
   </si>
   <si>
@@ -90,9 +84,6 @@
     <t>Tagplade</t>
   </si>
   <si>
-    <t>Alle tal er i mm hvis ikke andet er angivet</t>
-  </si>
-  <si>
     <t>Rejsning</t>
   </si>
   <si>
@@ -111,18 +102,12 @@
     <t>Tagsten dobbelt -s sort</t>
   </si>
   <si>
-    <t>carport længde / 400</t>
-  </si>
-  <si>
     <t>Rygstensbeslag</t>
   </si>
   <si>
     <t>Belædningsplader skur</t>
   </si>
   <si>
-    <t>((carport længde x bredde) / 1000000) * 14</t>
-  </si>
-  <si>
     <t>Rygstenen er 420 mm og skal overlappe med 10 mm. Derfor skal der bruges 2,5 rygsten pr. 1000 mm carport i længden</t>
   </si>
   <si>
@@ -135,12 +120,6 @@
     <t>Antal</t>
   </si>
   <si>
-    <t>900 + carport højde</t>
-  </si>
-  <si>
-    <t>((skur længde / 60) x 2) + ((skur bredde / 60) x 2))</t>
-  </si>
-  <si>
     <t>z til bagside af dør i skur</t>
   </si>
   <si>
@@ -153,21 +132,12 @@
     <t>Løsholter til skur gavle</t>
   </si>
   <si>
-    <t>1 x skur bredde</t>
-  </si>
-  <si>
-    <t>1 x skur længde</t>
-  </si>
-  <si>
     <t>Spær</t>
   </si>
   <si>
     <t>Færdigsamlet spær</t>
   </si>
   <si>
-    <t>carport længde / 1000</t>
-  </si>
-  <si>
     <t>Kategori</t>
   </si>
   <si>
@@ -177,24 +147,12 @@
     <t>Tagpakken</t>
   </si>
   <si>
-    <t>1 x carport længde</t>
-  </si>
-  <si>
-    <t>1 x carport bredde</t>
-  </si>
-  <si>
     <t>Beslag &amp; skruer</t>
   </si>
   <si>
     <t>Skruer til tagplader</t>
   </si>
   <si>
-    <t>(carport længde x bredde) / 1000000 / 15</t>
-  </si>
-  <si>
-    <t>Plastmo tag på carport</t>
-  </si>
-  <si>
     <t>Vindkryds på spær</t>
   </si>
   <si>
@@ -225,18 +183,12 @@
     <t>Plastmo bundskruer 200 stk.</t>
   </si>
   <si>
-    <t>(carport længde x bredde) / 1000000 / 25</t>
-  </si>
-  <si>
     <t>Der skal bruges 1 stk. pr. 25 m2 carport</t>
   </si>
   <si>
     <t>Der skal bruges 1 pakke pr. 15 m2 tag</t>
   </si>
   <si>
-    <t>carport længde / 500</t>
-  </si>
-  <si>
     <t>Forbrug er 2 pr. meter carport længde</t>
   </si>
   <si>
@@ -258,9 +210,6 @@
     <t>4,5x60 mm. skruer 200 stk.</t>
   </si>
   <si>
-    <t>((carport længde + 600) x (bredde+600)) / 1000000)</t>
-  </si>
-  <si>
     <t>Plader overlapper med 200 mm. så forbrug = 1 plade per m2. Derudover er der 300 mm. udhæng på alle sider</t>
   </si>
   <si>
@@ -270,48 +219,27 @@
     <t>Spær monteres med 550 mm mellemrum hvis taget er fladt</t>
   </si>
   <si>
-    <t>carport længde / 550</t>
-  </si>
-  <si>
     <t>Beslag til spær på rem</t>
   </si>
   <si>
     <t>Skruer til universalbeslag + hulbånd</t>
   </si>
   <si>
-    <t>Forbruget af spær er 1 stk. pr. 55 mm længde carport. Forbrug af beslag pr. spær er 2 stk. Forbruger af skruer pr. beslag er 4 stk. Derudover forbruges der 100 skruer pr. hulbånd.</t>
-  </si>
-  <si>
-    <t>((((carport længde / 550) x 2) x 4) +  (((carport længde x bredde) / 1000000 / 25) x 100)</t>
-  </si>
-  <si>
-    <t>Skruer til montering af stern, vindskeder og vandbræt</t>
-  </si>
-  <si>
     <t>1 pakke skruer pr. 25 m2 carport</t>
   </si>
   <si>
     <t>Universal 190 mm venstre</t>
   </si>
   <si>
-    <t>(1 x carport højde) - 200</t>
-  </si>
-  <si>
     <t xml:space="preserve">Plader monteres 1 på 2 med 20 mm overlap i hver side. </t>
   </si>
   <si>
-    <t xml:space="preserve">10 stolper pr. skur. 900 mm nedgravet pr. stolpe. </t>
-  </si>
-  <si>
     <t>Forbrug er 2 stk. pr. stolpe</t>
   </si>
   <si>
     <t>Løsholter er dem som belægningspladerne til skuret skrues ind i i bunden</t>
   </si>
   <si>
-    <t>Pris i DKK</t>
-  </si>
-  <si>
     <t>Til lås på dør i skur</t>
   </si>
   <si>
@@ -336,9 +264,6 @@
     <t>Minimum 4 stk. og yderligere 1 pr. m2 skur</t>
   </si>
   <si>
-    <t>((skur længde x bredde) / 1000000) + 4</t>
-  </si>
-  <si>
     <t>4,5 x 70 mm. skruer 400 stk.</t>
   </si>
   <si>
@@ -354,18 +279,6 @@
     <t>ID</t>
   </si>
   <si>
-    <t>Antal beklædningsbrædder / 2 da kun hver andet bredt er yderst.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">((skur længde / 60) x 2) + ((skur bredde / 60) x 2)) / 2 </t>
-  </si>
-  <si>
-    <t>(((skur længde / 60) x 2) + ((skur bredde / 60) x 2)) / 2) x 2</t>
-  </si>
-  <si>
-    <t>Antal beklædningsbrædder / 2 da kun hver andet bredt er inderst men x 2 til sidst da der skal to  skruer pr. inderste beklædningsbræt</t>
-  </si>
-  <si>
     <t>Toplægte holder</t>
   </si>
   <si>
@@ -402,9 +315,6 @@
     <t>Taget antages samme højde/hældning uanset hvad. Så eneste faktor er bredden.</t>
   </si>
   <si>
-    <t>1,4 x carport bredde</t>
-  </si>
-  <si>
     <t>38x73 mm. Taglægte T1</t>
   </si>
   <si>
@@ -441,10 +351,107 @@
     <t>Trapez plast sort</t>
   </si>
   <si>
-    <t>300 + carport længde</t>
-  </si>
-  <si>
     <t>300 mm udhæng i hver ende og et bræt på hver side.</t>
+  </si>
+  <si>
+    <t>carport l / 550</t>
+  </si>
+  <si>
+    <t>carport l / 1000</t>
+  </si>
+  <si>
+    <t>carport l / 400</t>
+  </si>
+  <si>
+    <t>carport l / 500</t>
+  </si>
+  <si>
+    <t>((skur l / 60) x 2) + ((skur b / 60) x 2))</t>
+  </si>
+  <si>
+    <t>((carport l + 600) x (b+600)) / 1000000)</t>
+  </si>
+  <si>
+    <t>((carport l x b) / 1000000) * 14</t>
+  </si>
+  <si>
+    <t>(carport l x b) / 1000000 / 15</t>
+  </si>
+  <si>
+    <t>(carport l x b) / 1000000 / 25</t>
+  </si>
+  <si>
+    <t>((((carport l / 550) x 2) x 4) +  (((carport l x b) / 1000000 / 25) x 100)</t>
+  </si>
+  <si>
+    <t>((skur l x b) / 1000000) + 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">((skur l / 60) x 2) + ((skur b / 60) x 2)) / 2 </t>
+  </si>
+  <si>
+    <t>(((skur l / 60) x 2) + ((skur b / 60) x 2)) / 2) x 2</t>
+  </si>
+  <si>
+    <t>Carport l &lt; 4800</t>
+  </si>
+  <si>
+    <t>Carport l &gt; 4800</t>
+  </si>
+  <si>
+    <t>Tag = Plastmo</t>
+  </si>
+  <si>
+    <t>Montering af stern, vindskeder og vandbræt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8 stolper pr. skur. 900 mm nedgravet pr. stolpe. </t>
+  </si>
+  <si>
+    <t>1 stk. pr. skur uanset hvad.</t>
+  </si>
+  <si>
+    <t>Kun et bræt foran i samme bredde som skuret.</t>
+  </si>
+  <si>
+    <t>2 remme uanset hvad, og i samme længde som carporten.</t>
+  </si>
+  <si>
+    <t>1 stk. spær pr. 55 mm l carport. 2 stk. beslag pr. spær. 4 skruer pr. beslag. Derudover 100 skruer pr. hulbånd.</t>
+  </si>
+  <si>
+    <t>Antal beklædningsbrædder / 2 da kun hver andet bræt er yderst.</t>
+  </si>
+  <si>
+    <t>Antal beklædningsbrædder / 2 da kun hver andet bræt er inderst men x 2, da der skal to  skruer pr. inderste beklædningsbræt</t>
+  </si>
+  <si>
+    <t>300 + carport l</t>
+  </si>
+  <si>
+    <t>1 x carport l</t>
+  </si>
+  <si>
+    <t>1 x skur l</t>
+  </si>
+  <si>
+    <t>1 x carport b</t>
+  </si>
+  <si>
+    <t>1 x skur b</t>
+  </si>
+  <si>
+    <t>1,4 x carport b</t>
+  </si>
+  <si>
+    <t>900 + carport h</t>
+  </si>
+  <si>
+    <t>(1 x carport h) - 200</t>
+  </si>
+  <si>
+    <t>Alle tal er i mm hvis ikke andet er angivet.
+l = længde, b = bredde og h = højde.</t>
   </si>
 </sst>
 </file>
@@ -509,7 +516,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -550,6 +557,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -868,31 +878,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5399CBF3-4BE6-4B04-A481-78794DB7A6C6}">
-  <dimension ref="A1:L47"/>
+  <dimension ref="A1:K47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:K47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="2.33203125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="7.109375" style="4" customWidth="1"/>
-    <col min="3" max="3" width="20.77734375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="4.88671875" style="4" customWidth="1"/>
+    <col min="3" max="3" width="13.88671875" style="1" customWidth="1"/>
     <col min="4" max="4" width="9.44140625" style="1" customWidth="1"/>
     <col min="5" max="5" width="7.44140625" style="1" customWidth="1"/>
     <col min="6" max="6" width="14.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="44.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="35.5546875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="22.77734375" style="1" customWidth="1"/>
-    <col min="10" max="10" width="75.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13" style="1" customWidth="1"/>
-    <col min="12" max="12" width="121.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.77734375" customWidth="1"/>
-    <col min="14" max="14" width="9.21875" customWidth="1"/>
+    <col min="7" max="7" width="36.33203125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="33" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="55.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="103.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.77734375" customWidth="1"/>
+    <col min="13" max="13" width="9.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B1" s="5"/>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
@@ -903,31 +912,29 @@
       <c r="I1" s="3"/>
       <c r="J1" s="3"/>
       <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-    </row>
-    <row r="2" spans="1:12" s="7" customFormat="1" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:11" s="7" customFormat="1" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6"/>
       <c r="B2" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
-      <c r="I2" s="15"/>
+        <v>138</v>
+      </c>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16"/>
+      <c r="I2" s="16"/>
       <c r="J2" s="11"/>
-      <c r="K2" s="11"/>
-      <c r="L2" s="9"/>
-    </row>
-    <row r="3" spans="1:12" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K2" s="9"/>
+    </row>
+    <row r="3" spans="1:11" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6"/>
       <c r="B3" s="14" t="s">
-        <v>105</v>
+        <v>80</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>11</v>
@@ -936,7 +943,7 @@
         <v>10</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="G3" s="8" t="s">
         <v>6</v>
@@ -945,19 +952,16 @@
         <v>7</v>
       </c>
       <c r="I3" s="8" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="J3" s="8" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="K3" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="L3" s="8" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="6"/>
       <c r="B4" s="12">
         <v>1</v>
@@ -972,28 +976,25 @@
         <v>1</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="G4" s="9" t="s">
         <v>8</v>
       </c>
       <c r="H4" s="9" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="I4" s="9" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="J4" s="9">
         <v>2</v>
       </c>
       <c r="K4" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="L4" s="9" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="6"/>
       <c r="B5" s="12">
         <v>2</v>
@@ -1008,34 +1009,31 @@
         <v>1</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="G5" s="9" t="s">
         <v>9</v>
       </c>
       <c r="H5" s="9" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="I5" s="9" t="s">
-        <v>48</v>
+        <v>133</v>
       </c>
       <c r="J5" s="9">
         <v>1</v>
       </c>
       <c r="K5" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="L5" s="9" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="6"/>
       <c r="B6" s="12">
         <v>3</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>13</v>
+        <v>119</v>
       </c>
       <c r="D6" s="9" t="s">
         <v>1</v>
@@ -1044,34 +1042,31 @@
         <v>4</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="G6" s="9" t="s">
         <v>0</v>
       </c>
       <c r="H6" s="9" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="I6" s="9" t="s">
-        <v>33</v>
+        <v>136</v>
       </c>
       <c r="J6" s="9">
         <v>4</v>
       </c>
       <c r="K6" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="L6" s="9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="6"/>
       <c r="B7" s="12">
         <v>3</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>12</v>
+        <v>120</v>
       </c>
       <c r="D7" s="9" t="s">
         <v>1</v>
@@ -1080,28 +1075,25 @@
         <v>4</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="G7" s="9" t="s">
         <v>0</v>
       </c>
       <c r="H7" s="9" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="I7" s="9" t="s">
-        <v>33</v>
+        <v>136</v>
       </c>
       <c r="J7" s="9">
         <v>6</v>
       </c>
       <c r="K7" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="L7" s="9" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="6"/>
       <c r="B8" s="12">
         <v>3</v>
@@ -1116,28 +1108,25 @@
         <v>5</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="G8" s="9" t="s">
         <v>0</v>
       </c>
       <c r="H8" s="9" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="I8" s="9" t="s">
-        <v>33</v>
+        <v>136</v>
       </c>
       <c r="J8" s="9">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="K8" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="L8" s="9" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="6"/>
       <c r="B9" s="12">
         <v>4</v>
@@ -1152,28 +1141,25 @@
         <v>5</v>
       </c>
       <c r="F9" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="H9" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="G9" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="H9" s="9" t="s">
-        <v>59</v>
-      </c>
       <c r="I9" s="9" t="s">
-        <v>86</v>
+        <v>137</v>
       </c>
       <c r="J9" s="10" t="s">
-        <v>34</v>
+        <v>110</v>
       </c>
       <c r="K9" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="L9" s="9" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="6"/>
       <c r="B10" s="12">
         <v>5</v>
@@ -1188,13 +1174,13 @@
         <v>5</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="G10" s="9" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="H10" s="9" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="I10" s="9">
         <v>420</v>
@@ -1203,13 +1189,10 @@
         <v>1</v>
       </c>
       <c r="K10" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="L10" s="9" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="6"/>
       <c r="B11" s="12">
         <v>6</v>
@@ -1224,28 +1207,25 @@
         <v>1</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="G11" s="9" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="H11" s="9" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
       <c r="I11" s="9" t="s">
-        <v>47</v>
+        <v>131</v>
       </c>
       <c r="J11" s="9">
         <v>2</v>
       </c>
       <c r="K11" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="L11" s="9" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="6"/>
       <c r="B12" s="12">
         <v>7</v>
@@ -1260,28 +1240,25 @@
         <v>1</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="H12" s="9" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
       <c r="I12" s="9" t="s">
-        <v>48</v>
+        <v>133</v>
       </c>
       <c r="J12" s="9" t="s">
-        <v>78</v>
+        <v>106</v>
       </c>
       <c r="K12" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="L12" s="9" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="6"/>
       <c r="B13" s="12">
         <v>8</v>
@@ -1296,28 +1273,25 @@
         <v>5</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="G13" s="9" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="H13" s="9" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
       <c r="I13" s="9" t="s">
-        <v>40</v>
+        <v>132</v>
       </c>
       <c r="J13" s="9">
         <v>2</v>
       </c>
       <c r="K13" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="L13" s="9" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="6"/>
       <c r="B14" s="12">
         <v>9</v>
@@ -1332,28 +1306,25 @@
         <v>5</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="G14" s="9" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="H14" s="9" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
       <c r="I14" s="9" t="s">
-        <v>39</v>
+        <v>134</v>
       </c>
       <c r="J14" s="9">
         <v>2</v>
       </c>
       <c r="K14" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="L14" s="9" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="6"/>
       <c r="B15" s="12">
         <v>10</v>
@@ -1362,34 +1333,31 @@
         <v>3</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E15" s="9" t="s">
         <v>1</v>
       </c>
       <c r="F15" s="9" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="G15" s="9" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="H15" s="9" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="I15" s="9">
         <v>0</v>
       </c>
       <c r="J15" s="9" t="s">
-        <v>43</v>
+        <v>107</v>
       </c>
       <c r="K15" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="L15" s="9" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="6"/>
       <c r="B16" s="12">
         <v>11</v>
@@ -1398,34 +1366,31 @@
         <v>3</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E16" s="9" t="s">
         <v>1</v>
       </c>
       <c r="F16" s="9" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="G16" s="9" t="s">
-        <v>119</v>
+        <v>90</v>
       </c>
       <c r="H16" s="9" t="s">
-        <v>120</v>
+        <v>91</v>
       </c>
       <c r="I16" s="9" t="s">
-        <v>122</v>
+        <v>135</v>
       </c>
       <c r="J16" s="9">
         <v>2</v>
       </c>
       <c r="K16" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="L16" s="9" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="6"/>
       <c r="B17" s="12">
         <v>12</v>
@@ -1434,34 +1399,31 @@
         <v>3</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E17" s="9" t="s">
         <v>1</v>
       </c>
       <c r="F17" s="9" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="G17" s="9" t="s">
-        <v>123</v>
+        <v>93</v>
       </c>
       <c r="H17" s="9" t="s">
-        <v>125</v>
+        <v>95</v>
       </c>
       <c r="I17" s="9">
         <v>540</v>
       </c>
       <c r="J17" s="9" t="s">
-        <v>43</v>
+        <v>107</v>
       </c>
       <c r="K17" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="L17" s="9" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="6"/>
       <c r="B18" s="12">
         <v>13</v>
@@ -1470,34 +1432,31 @@
         <v>3</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E18" s="9" t="s">
         <v>1</v>
       </c>
       <c r="F18" s="9" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="G18" s="9" t="s">
-        <v>123</v>
+        <v>93</v>
       </c>
       <c r="H18" s="9" t="s">
-        <v>126</v>
+        <v>96</v>
       </c>
       <c r="I18" s="9" t="s">
-        <v>47</v>
+        <v>131</v>
       </c>
       <c r="J18" s="9">
         <v>1</v>
       </c>
       <c r="K18" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="L18" s="9" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="6"/>
       <c r="B19" s="12">
         <v>14</v>
@@ -1512,28 +1471,25 @@
         <v>1</v>
       </c>
       <c r="F19" s="9" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="G19" s="9" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H19" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="I19" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="J19" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="K19" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="I19" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="J19" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="K19" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="L19" s="9" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="1:11" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="6"/>
       <c r="B20" s="12">
         <v>15</v>
@@ -1542,34 +1498,31 @@
         <v>3</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E20" s="9" t="s">
         <v>1</v>
       </c>
       <c r="F20" s="9" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="G20" s="9" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="H20" s="9" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="I20" s="9" t="s">
         <v>3</v>
       </c>
       <c r="J20" s="9" t="s">
-        <v>28</v>
+        <v>112</v>
       </c>
       <c r="K20" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="L20" s="9" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="6"/>
       <c r="B21" s="12">
         <v>16</v>
@@ -1578,34 +1531,31 @@
         <v>3</v>
       </c>
       <c r="D21" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E21" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="F21" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="G21" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="E21" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="F21" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="G21" s="13" t="s">
-        <v>22</v>
-      </c>
       <c r="H21" s="9" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="I21" s="9" t="s">
         <v>3</v>
       </c>
       <c r="J21" s="9" t="s">
-        <v>25</v>
+        <v>108</v>
       </c>
       <c r="K21" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="L21" s="9" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="6"/>
       <c r="B22" s="12">
         <v>17</v>
@@ -1614,40 +1564,37 @@
         <v>3</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E22" s="9" t="s">
         <v>1</v>
       </c>
       <c r="F22" s="9" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="G22" s="9" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="H22" s="9" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="I22" s="9" t="s">
         <v>3</v>
       </c>
       <c r="J22" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="K22" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="K22" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="L22" s="9" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="23" spans="1:11" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="6"/>
       <c r="B23" s="12">
         <v>18</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>52</v>
+        <v>121</v>
       </c>
       <c r="D23" s="9" t="s">
         <v>2</v>
@@ -1656,28 +1603,25 @@
         <v>1</v>
       </c>
       <c r="F23" s="9" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="G23" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="H23" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="I23" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="J23" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="K23" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="H23" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="I23" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="J23" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="K23" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="L23" s="9" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="24" spans="1:11" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="6"/>
       <c r="B24" s="12">
         <v>19</v>
@@ -1686,34 +1630,31 @@
         <v>3</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E24" s="9" t="s">
         <v>1</v>
       </c>
       <c r="F24" s="9" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="G24" s="9" t="s">
-        <v>112</v>
+        <v>83</v>
       </c>
       <c r="H24" s="9" t="s">
-        <v>110</v>
+        <v>81</v>
       </c>
       <c r="I24" s="9" t="s">
         <v>3</v>
       </c>
       <c r="J24" s="9" t="s">
-        <v>43</v>
+        <v>107</v>
       </c>
       <c r="K24" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="L24" s="9" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="6"/>
       <c r="B25" s="12">
         <v>20</v>
@@ -1722,34 +1663,31 @@
         <v>3</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E25" s="9" t="s">
         <v>1</v>
       </c>
       <c r="F25" s="9" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="G25" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="H25" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="I25" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="J25" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="H25" s="9" t="s">
-        <v>114</v>
-      </c>
-      <c r="I25" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="J25" s="9" t="s">
-        <v>51</v>
-      </c>
       <c r="K25" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="L25" s="9" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="6"/>
       <c r="B26" s="12">
         <v>21</v>
@@ -1758,34 +1696,31 @@
         <v>3</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E26" s="9" t="s">
         <v>1</v>
       </c>
       <c r="F26" s="9" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="G26" s="9" t="s">
-        <v>117</v>
+        <v>88</v>
       </c>
       <c r="H26" s="9" t="s">
-        <v>118</v>
+        <v>89</v>
       </c>
       <c r="I26" s="9" t="s">
         <v>3</v>
       </c>
       <c r="J26" s="9" t="s">
-        <v>51</v>
+        <v>113</v>
       </c>
       <c r="K26" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="L26" s="9" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="6"/>
       <c r="B27" s="12">
         <v>22</v>
@@ -1800,28 +1735,25 @@
         <v>1</v>
       </c>
       <c r="F27" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="G27" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="H27" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="I27" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="J27" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="K27" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="G27" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="H27" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="I27" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="J27" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="K27" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="L27" s="9" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="28" spans="1:11" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="6"/>
       <c r="B28" s="12">
         <v>23</v>
@@ -1836,28 +1768,25 @@
         <v>1</v>
       </c>
       <c r="F28" s="9" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="G28" s="9" t="s">
-        <v>79</v>
+        <v>61</v>
       </c>
       <c r="H28" s="9" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
       <c r="I28" s="9" t="s">
         <v>3</v>
       </c>
       <c r="J28" s="9" t="s">
-        <v>66</v>
+        <v>109</v>
       </c>
       <c r="K28" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="L28" s="9" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="6"/>
       <c r="B29" s="12">
         <v>24</v>
@@ -1872,28 +1801,25 @@
         <v>1</v>
       </c>
       <c r="F29" s="9" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="G29" s="9" t="s">
-        <v>79</v>
+        <v>61</v>
       </c>
       <c r="H29" s="9" t="s">
-        <v>85</v>
+        <v>64</v>
       </c>
       <c r="I29" s="9" t="s">
         <v>3</v>
       </c>
       <c r="J29" s="9" t="s">
-        <v>66</v>
+        <v>109</v>
       </c>
       <c r="K29" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="L29" s="9" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="6"/>
       <c r="B30" s="12">
         <v>25</v>
@@ -1908,34 +1834,31 @@
         <v>1</v>
       </c>
       <c r="F30" s="9" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="G30" s="9" t="s">
-        <v>80</v>
+        <v>62</v>
       </c>
       <c r="H30" s="9" t="s">
-        <v>94</v>
+        <v>70</v>
       </c>
       <c r="I30" s="9" t="s">
         <v>3</v>
       </c>
       <c r="J30" s="9" t="s">
-        <v>82</v>
+        <v>115</v>
       </c>
       <c r="K30" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="L30" s="9" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="6"/>
       <c r="B31" s="12">
         <v>26</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>13</v>
+        <v>119</v>
       </c>
       <c r="D31" s="9" t="s">
         <v>1</v>
@@ -1944,13 +1867,13 @@
         <v>4</v>
       </c>
       <c r="F31" s="9" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="G31" s="9" t="s">
-        <v>70</v>
+        <v>54</v>
       </c>
       <c r="H31" s="9" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
       <c r="I31" s="9" t="s">
         <v>3</v>
@@ -1959,19 +1882,16 @@
         <v>8</v>
       </c>
       <c r="K31" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="L31" s="9" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="6"/>
       <c r="B32" s="12">
         <v>26</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>12</v>
+        <v>120</v>
       </c>
       <c r="D32" s="9" t="s">
         <v>1</v>
@@ -1980,13 +1900,13 @@
         <v>4</v>
       </c>
       <c r="F32" s="9" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="G32" s="9" t="s">
-        <v>70</v>
+        <v>54</v>
       </c>
       <c r="H32" s="9" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
       <c r="I32" s="9" t="s">
         <v>3</v>
@@ -1995,13 +1915,10 @@
         <v>12</v>
       </c>
       <c r="K32" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="L32" s="9" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="6"/>
       <c r="B33" s="12">
         <v>26</v>
@@ -2016,34 +1933,31 @@
         <v>5</v>
       </c>
       <c r="F33" s="9" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="G33" s="9" t="s">
-        <v>70</v>
+        <v>54</v>
       </c>
       <c r="H33" s="9" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
       <c r="I33" s="9" t="s">
         <v>3</v>
       </c>
       <c r="J33" s="9">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="K33" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="L33" s="9" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="6"/>
       <c r="B34" s="12">
         <v>27</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>13</v>
+        <v>119</v>
       </c>
       <c r="D34" s="9" t="s">
         <v>1</v>
@@ -2052,13 +1966,13 @@
         <v>4</v>
       </c>
       <c r="F34" s="9" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="G34" s="9" t="s">
-        <v>70</v>
+        <v>54</v>
       </c>
       <c r="H34" s="9" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="I34" s="9" t="s">
         <v>3</v>
@@ -2067,19 +1981,16 @@
         <v>8</v>
       </c>
       <c r="K34" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="L34" s="9" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="6"/>
       <c r="B35" s="12">
         <v>27</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>12</v>
+        <v>120</v>
       </c>
       <c r="D35" s="9" t="s">
         <v>1</v>
@@ -2088,13 +1999,13 @@
         <v>4</v>
       </c>
       <c r="F35" s="9" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="G35" s="9" t="s">
-        <v>70</v>
+        <v>54</v>
       </c>
       <c r="H35" s="9" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="I35" s="9" t="s">
         <v>3</v>
@@ -2103,13 +2014,10 @@
         <v>12</v>
       </c>
       <c r="K35" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="L35" s="9" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="6"/>
       <c r="B36" s="12">
         <v>27</v>
@@ -2124,28 +2032,25 @@
         <v>5</v>
       </c>
       <c r="F36" s="9" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="G36" s="9" t="s">
-        <v>70</v>
+        <v>54</v>
       </c>
       <c r="H36" s="9" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="I36" s="9" t="s">
         <v>3</v>
       </c>
       <c r="J36" s="9">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="K36" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="L36" s="9" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="6"/>
       <c r="B37" s="12">
         <v>28</v>
@@ -2160,28 +2065,25 @@
         <v>1</v>
       </c>
       <c r="F37" s="9" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="G37" s="9" t="s">
-        <v>83</v>
+        <v>122</v>
       </c>
       <c r="H37" s="9" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
       <c r="I37" s="9" t="s">
         <v>3</v>
       </c>
       <c r="J37" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="K37" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="K37" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="L37" s="9" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="38" spans="1:11" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="6"/>
       <c r="B38" s="12">
         <v>29</v>
@@ -2196,13 +2098,13 @@
         <v>5</v>
       </c>
       <c r="F38" s="9" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="G38" s="9" t="s">
-        <v>92</v>
+        <v>68</v>
       </c>
       <c r="H38" s="9" t="s">
-        <v>93</v>
+        <v>69</v>
       </c>
       <c r="I38" s="9" t="s">
         <v>3</v>
@@ -2211,13 +2113,10 @@
         <v>1</v>
       </c>
       <c r="K38" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="L38" s="9" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="6"/>
       <c r="B39" s="12">
         <v>30</v>
@@ -2232,13 +2131,13 @@
         <v>5</v>
       </c>
       <c r="F39" s="9" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="G39" s="9" t="s">
-        <v>96</v>
+        <v>72</v>
       </c>
       <c r="H39" s="9" t="s">
-        <v>95</v>
+        <v>71</v>
       </c>
       <c r="I39" s="9" t="s">
         <v>3</v>
@@ -2247,13 +2146,10 @@
         <v>1</v>
       </c>
       <c r="K39" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="L39" s="9" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="6"/>
       <c r="B40" s="12">
         <v>31</v>
@@ -2268,28 +2164,25 @@
         <v>5</v>
       </c>
       <c r="F40" s="9" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="G40" s="9" t="s">
-        <v>97</v>
+        <v>73</v>
       </c>
       <c r="H40" s="9" t="s">
-        <v>98</v>
+        <v>74</v>
       </c>
       <c r="I40" s="9" t="s">
         <v>3</v>
       </c>
       <c r="J40" s="9" t="s">
-        <v>100</v>
+        <v>116</v>
       </c>
       <c r="K40" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="L40" s="9" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="6"/>
       <c r="B41" s="12">
         <v>32</v>
@@ -2304,28 +2197,25 @@
         <v>5</v>
       </c>
       <c r="F41" s="9" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="G41" s="9" t="s">
-        <v>103</v>
+        <v>78</v>
       </c>
       <c r="H41" s="9" t="s">
-        <v>101</v>
+        <v>76</v>
       </c>
       <c r="I41" s="9" t="s">
         <v>3</v>
       </c>
       <c r="J41" s="10" t="s">
-        <v>107</v>
+        <v>117</v>
       </c>
       <c r="K41" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="L41" s="9" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="6"/>
       <c r="B42" s="12">
         <v>33</v>
@@ -2340,28 +2230,25 @@
         <v>5</v>
       </c>
       <c r="F42" s="9" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="G42" s="9" t="s">
-        <v>104</v>
+        <v>79</v>
       </c>
       <c r="H42" s="9" t="s">
-        <v>102</v>
+        <v>77</v>
       </c>
       <c r="I42" s="9" t="s">
         <v>3</v>
       </c>
       <c r="J42" s="10" t="s">
-        <v>108</v>
+        <v>118</v>
       </c>
       <c r="K42" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="L42" s="9" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="43" spans="1:12" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="6"/>
       <c r="B43" s="12">
         <v>34</v>
@@ -2376,28 +2263,25 @@
         <v>1</v>
       </c>
       <c r="F43" s="9" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="G43" s="9" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H43" s="9" t="s">
-        <v>129</v>
+        <v>99</v>
       </c>
       <c r="I43" s="9" t="s">
         <v>3</v>
       </c>
       <c r="J43" s="9" t="s">
-        <v>74</v>
+        <v>111</v>
       </c>
       <c r="K43" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="L43" s="9" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="44" spans="1:12" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="6"/>
       <c r="B44" s="12">
         <v>35</v>
@@ -2412,28 +2296,25 @@
         <v>1</v>
       </c>
       <c r="F44" s="9" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="G44" s="9" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H44" s="9" t="s">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="I44" s="9" t="s">
         <v>3</v>
       </c>
       <c r="J44" s="9" t="s">
-        <v>74</v>
+        <v>111</v>
       </c>
       <c r="K44" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="L44" s="9" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="45" spans="1:12" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="6"/>
       <c r="B45" s="12">
         <v>36</v>
@@ -2448,28 +2329,25 @@
         <v>1</v>
       </c>
       <c r="F45" s="9" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="G45" s="9" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H45" s="9" t="s">
-        <v>131</v>
+        <v>101</v>
       </c>
       <c r="I45" s="9" t="s">
         <v>3</v>
       </c>
       <c r="J45" s="9" t="s">
-        <v>74</v>
+        <v>111</v>
       </c>
       <c r="K45" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="L45" s="9" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="46" spans="1:12" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="6"/>
       <c r="B46" s="12">
         <v>37</v>
@@ -2478,34 +2356,31 @@
         <v>3</v>
       </c>
       <c r="D46" s="9" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E46" s="9" t="s">
         <v>1</v>
       </c>
       <c r="F46" s="9" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="G46" s="9" t="s">
-        <v>133</v>
+        <v>103</v>
       </c>
       <c r="H46" s="9" t="s">
-        <v>132</v>
+        <v>102</v>
       </c>
       <c r="I46" s="9" t="s">
         <v>3</v>
       </c>
       <c r="J46" s="9" t="s">
-        <v>28</v>
+        <v>112</v>
       </c>
       <c r="K46" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="L46" s="9" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="47" spans="1:12" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="6"/>
       <c r="B47" s="12">
         <v>38</v>
@@ -2514,36 +2389,33 @@
         <v>3</v>
       </c>
       <c r="D47" s="9" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E47" s="9" t="s">
         <v>1</v>
       </c>
       <c r="F47" s="9" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="G47" s="9" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H47" s="9" t="s">
-        <v>134</v>
+        <v>104</v>
       </c>
       <c r="I47" s="9" t="s">
         <v>3</v>
       </c>
       <c r="J47" s="9" t="s">
-        <v>28</v>
+        <v>112</v>
       </c>
       <c r="K47" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="L47" s="9" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B3:L47" xr:uid="{1CB78581-2663-43A3-A1D3-214D99459CF7}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B4:L42">
+  <autoFilter ref="B3:K47" xr:uid="{1CB78581-2663-43A3-A1D3-214D99459CF7}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B4:K42">
       <sortCondition descending="1" ref="F3:F36"/>
     </sortState>
   </autoFilter>

</xml_diff>

<commit_message>
Diverse ændringer som vi har lavet sammen over Zoom
</commit_message>
<xml_diff>
--- a/documents/Materialeliste beregninger.xlsx
+++ b/documents/Materialeliste beregninger.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bruger\Desktop\2 SEM eksamen\Fog\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8504F5E4-D5F5-44A4-9A99-7A0DE3F5A886}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93ACB665-C494-4E82-B212-5FA75102AE6E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{02919F5A-1519-4947-A4AE-EA2FF4BD8D19}"/>
+    <workbookView xWindow="1128" yWindow="948" windowWidth="23040" windowHeight="12216" xr2:uid="{02919F5A-1519-4947-A4AE-EA2FF4BD8D19}"/>
   </bookViews>
   <sheets>
     <sheet name="Alt" sheetId="1" r:id="rId1"/>
@@ -880,8 +880,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5399CBF3-4BE6-4B04-A481-78794DB7A6C6}">
   <dimension ref="A1:K47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:K47"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>